<commit_message>
Generacion libro diario a excel v1
</commit_message>
<xml_diff>
--- a/app/templates/contable/plantillas/L,D.xlsx
+++ b/app/templates/contable/plantillas/L,D.xlsx
@@ -1,16 +1,16 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
 <workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="24326"/>
+  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="28129"/>
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="https://d.docs.live.net/4b7f090fe45a08e7/Escritorio/Curso de Contab. y Finanzas 2021 - II/Sesiones Contab. - Ing. Sistemas 2021 -II/"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angel\OneDrive\Imágenes\Escritorio\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="3" documentId="11_205142F29315A21D1D26A8F4EF2A2F94183AAD08" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{D3A805B9-A157-415D-AB2A-C7372A0DC6FB}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9A6DEBD-5A02-4485-8D41-5BAF5394F0E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
-    <workbookView xWindow="-120" yWindow="-120" windowWidth="20730" windowHeight="11160" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
   <sheets>
     <sheet name="Hoja1" sheetId="1" r:id="rId1"/>
@@ -25,7 +25,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="20" uniqueCount="20">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="19" uniqueCount="19">
   <si>
     <t>FORMATO 5.1: "LIBRO DIARIO"</t>
   </si>
@@ -37,9 +37,6 @@
   </si>
   <si>
     <t>APELLIDOS Y NOMBRES, DENOMINACIÓN O RAZÓN SOCIAL:</t>
-  </si>
-  <si>
-    <t>TOTALES</t>
   </si>
   <si>
     <t>GLOSA O DESCRIPCIÓN DE LA OPERACIÓN</t>
@@ -203,7 +200,7 @@
       </patternFill>
     </fill>
   </fills>
-  <borders count="12">
+  <borders count="11">
     <border>
       <left/>
       <right/>
@@ -331,38 +328,29 @@
       </bottom>
       <diagonal/>
     </border>
-    <border>
-      <left/>
-      <right/>
-      <top style="thin">
-        <color indexed="64"/>
-      </top>
-      <bottom/>
-      <diagonal/>
-    </border>
   </borders>
   <cellStyleXfs count="2">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0"/>
     <xf numFmtId="164" fontId="11" fillId="0" borderId="0" applyFont="0" applyFill="0" applyBorder="0" applyAlignment="0" applyProtection="0"/>
   </cellStyleXfs>
-  <cellXfs count="45">
+  <cellXfs count="41">
     <xf numFmtId="0" fontId="0" fillId="0" borderId="0" xfId="0"/>
-    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="1" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="2" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
-    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="3" fillId="0" borderId="0" xfId="0" applyFont="1"/>
+    <xf numFmtId="0" fontId="5" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="6" fillId="0" borderId="0" xfId="0" applyFont="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1" applyFill="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="0" xfId="0" applyFont="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment vertical="center"/>
     </xf>
@@ -384,42 +372,36 @@
     <xf numFmtId="0" fontId="8" fillId="2" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="left" vertical="center"/>
     </xf>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="14" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="9" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="14" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="9" fillId="0" borderId="5" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1"/>
-    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyFill="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="9" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="7" fillId="0" borderId="1" xfId="0" applyFont="1" applyBorder="1"/>
+    <xf numFmtId="0" fontId="4" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="10" fillId="0" borderId="5" xfId="0" applyFont="1" applyBorder="1"/>
-    <xf numFmtId="17" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1"/>
+    <xf numFmtId="17" fontId="3" fillId="0" borderId="0" xfId="0" applyNumberFormat="1" applyFont="1"/>
     <xf numFmtId="164" fontId="9" fillId="0" borderId="9" xfId="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="14" fontId="12" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="14" fontId="12" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="49" fontId="12" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
+    <xf numFmtId="49" fontId="12" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center"/>
     </xf>
-    <xf numFmtId="3" fontId="7" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyFill="1" applyBorder="1"/>
-    <xf numFmtId="0" fontId="10" fillId="0" borderId="11" xfId="0" applyFont="1" applyBorder="1" applyAlignment="1">
-      <alignment horizontal="center"/>
-    </xf>
+    <xf numFmtId="3" fontId="7" fillId="0" borderId="9" xfId="0" applyNumberFormat="1" applyFont="1" applyBorder="1"/>
     <xf numFmtId="0" fontId="8" fillId="2" borderId="1" xfId="0" applyFont="1" applyFill="1" applyBorder="1" applyAlignment="1">
       <alignment horizontal="center" vertical="center" wrapText="1"/>
     </xf>
@@ -728,27 +710,27 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
-  <dimension ref="A1:J34"/>
+  <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="H1" sqref="H1"/>
+    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="D27" sqref="D27"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr baseColWidth="10" defaultRowHeight="15" x14ac:dyDescent="0.25"/>
+  <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
   <cols>
-    <col min="1" max="1" width="4.85546875" customWidth="1"/>
-    <col min="2" max="2" width="6.42578125" customWidth="1"/>
+    <col min="1" max="1" width="4.88671875" customWidth="1"/>
+    <col min="2" max="2" width="6.44140625" customWidth="1"/>
     <col min="3" max="3" width="28" customWidth="1"/>
-    <col min="4" max="4" width="6.5703125" customWidth="1"/>
-    <col min="5" max="5" width="5.7109375" customWidth="1"/>
-    <col min="6" max="6" width="11.5703125" customWidth="1"/>
-    <col min="7" max="7" width="7.28515625" customWidth="1"/>
-    <col min="8" max="8" width="49.140625" customWidth="1"/>
-    <col min="9" max="9" width="14.85546875" customWidth="1"/>
-    <col min="10" max="10" width="14.42578125" customWidth="1"/>
+    <col min="4" max="4" width="6.5546875" customWidth="1"/>
+    <col min="5" max="5" width="5.6640625" customWidth="1"/>
+    <col min="6" max="6" width="11.5546875" customWidth="1"/>
+    <col min="7" max="7" width="7.33203125" customWidth="1"/>
+    <col min="8" max="8" width="49.109375" customWidth="1"/>
+    <col min="9" max="9" width="14.88671875" customWidth="1"/>
+    <col min="10" max="10" width="14.44140625" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:10" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A1" s="1" t="s">
         <v>0</v>
       </c>
@@ -762,7 +744,7 @@
       <c r="I1" s="2"/>
       <c r="J1" s="2"/>
     </row>
-    <row r="2" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="2" spans="1:10" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A2" s="1"/>
       <c r="B2" s="1"/>
       <c r="C2" s="2"/>
@@ -774,12 +756,12 @@
       <c r="I2" s="2"/>
       <c r="J2" s="2"/>
     </row>
-    <row r="3" spans="1:10" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="3" spans="1:10" ht="21" x14ac:dyDescent="0.4">
       <c r="A3" s="4" t="s">
         <v>1</v>
       </c>
       <c r="B3" s="4"/>
-      <c r="C3" s="30"/>
+      <c r="C3" s="27"/>
       <c r="D3" s="3"/>
       <c r="E3" s="3"/>
       <c r="F3" s="5"/>
@@ -788,7 +770,7 @@
       <c r="I3" s="6"/>
       <c r="J3" s="6"/>
     </row>
-    <row r="4" spans="1:10" ht="20.25" x14ac:dyDescent="0.3">
+    <row r="4" spans="1:10" ht="21" x14ac:dyDescent="0.4">
       <c r="A4" s="4" t="s">
         <v>2</v>
       </c>
@@ -802,7 +784,7 @@
       <c r="I4" s="6"/>
       <c r="J4" s="6"/>
     </row>
-    <row r="5" spans="1:10" ht="23.25" x14ac:dyDescent="0.35">
+    <row r="5" spans="1:10" ht="22.8" x14ac:dyDescent="0.4">
       <c r="A5" s="4" t="s">
         <v>3</v>
       </c>
@@ -816,7 +798,7 @@
       <c r="I5" s="7"/>
       <c r="J5" s="7"/>
     </row>
-    <row r="6" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="6" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A6" s="5"/>
       <c r="B6" s="5"/>
       <c r="C6" s="5"/>
@@ -828,109 +810,109 @@
       <c r="I6" s="8"/>
       <c r="J6" s="8"/>
     </row>
-    <row r="7" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A7" s="36" t="s">
+    <row r="7" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A7" s="32" t="s">
+        <v>13</v>
+      </c>
+      <c r="B7" s="32" t="s">
+        <v>12</v>
+      </c>
+      <c r="C7" s="32" t="s">
+        <v>4</v>
+      </c>
+      <c r="D7" s="35" t="s">
+        <v>5</v>
+      </c>
+      <c r="E7" s="36"/>
+      <c r="F7" s="37"/>
+      <c r="G7" s="35" t="s">
+        <v>6</v>
+      </c>
+      <c r="H7" s="37"/>
+      <c r="I7" s="9" t="s">
         <v>14</v>
       </c>
-      <c r="B7" s="36" t="s">
-        <v>13</v>
-      </c>
-      <c r="C7" s="36" t="s">
-        <v>5</v>
-      </c>
-      <c r="D7" s="39" t="s">
-        <v>6</v>
-      </c>
-      <c r="E7" s="40"/>
-      <c r="F7" s="41"/>
-      <c r="G7" s="39" t="s">
+      <c r="J7" s="9"/>
+    </row>
+    <row r="8" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A8" s="33"/>
+      <c r="B8" s="33"/>
+      <c r="C8" s="33"/>
+      <c r="D8" s="32" t="s">
+        <v>11</v>
+      </c>
+      <c r="E8" s="32" t="s">
+        <v>15</v>
+      </c>
+      <c r="F8" s="32" t="s">
+        <v>16</v>
+      </c>
+      <c r="G8" s="38" t="s">
         <v>7</v>
       </c>
-      <c r="H7" s="41"/>
-      <c r="I7" s="9" t="s">
-        <v>15</v>
-      </c>
-      <c r="J7" s="9"/>
-    </row>
-    <row r="8" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A8" s="37"/>
-      <c r="B8" s="37"/>
-      <c r="C8" s="37"/>
-      <c r="D8" s="36" t="s">
-        <v>12</v>
-      </c>
-      <c r="E8" s="36" t="s">
-        <v>16</v>
-      </c>
-      <c r="F8" s="36" t="s">
-        <v>17</v>
-      </c>
-      <c r="G8" s="42" t="s">
+      <c r="H8" s="38" t="s">
         <v>8</v>
-      </c>
-      <c r="H8" s="42" t="s">
-        <v>9</v>
       </c>
       <c r="I8" s="10"/>
       <c r="J8" s="11"/>
     </row>
-    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.25">
-      <c r="A9" s="37"/>
-      <c r="B9" s="37"/>
-      <c r="C9" s="37"/>
-      <c r="D9" s="37"/>
-      <c r="E9" s="37"/>
-      <c r="F9" s="37"/>
-      <c r="G9" s="43"/>
-      <c r="H9" s="43"/>
+    <row r="9" spans="1:10" hidden="1" x14ac:dyDescent="0.3">
+      <c r="A9" s="33"/>
+      <c r="B9" s="33"/>
+      <c r="C9" s="33"/>
+      <c r="D9" s="33"/>
+      <c r="E9" s="33"/>
+      <c r="F9" s="33"/>
+      <c r="G9" s="39"/>
+      <c r="H9" s="39"/>
       <c r="I9" s="12" t="s">
+        <v>9</v>
+      </c>
+      <c r="J9" s="13" t="s">
         <v>10</v>
       </c>
-      <c r="J9" s="13" t="s">
-        <v>11</v>
-      </c>
-    </row>
-    <row r="10" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A10" s="38"/>
-      <c r="B10" s="38"/>
-      <c r="C10" s="38"/>
-      <c r="D10" s="38"/>
-      <c r="E10" s="38"/>
-      <c r="F10" s="38"/>
-      <c r="G10" s="44"/>
-      <c r="H10" s="44"/>
+    </row>
+    <row r="10" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A10" s="34"/>
+      <c r="B10" s="34"/>
+      <c r="C10" s="34"/>
+      <c r="D10" s="34"/>
+      <c r="E10" s="34"/>
+      <c r="F10" s="34"/>
+      <c r="G10" s="40"/>
+      <c r="H10" s="40"/>
       <c r="I10" s="14" t="s">
+        <v>17</v>
+      </c>
+      <c r="J10" s="15" t="s">
         <v>18</v>
       </c>
-      <c r="J10" s="15" t="s">
-        <v>19</v>
-      </c>
-    </row>
-    <row r="11" spans="1:10" x14ac:dyDescent="0.25">
+    </row>
+    <row r="11" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A11" s="16"/>
       <c r="B11" s="16"/>
-      <c r="C11" s="32"/>
-      <c r="D11" s="33"/>
-      <c r="E11" s="33"/>
-      <c r="F11" s="33"/>
-      <c r="G11" s="33"/>
-      <c r="H11" s="33"/>
+      <c r="C11" s="29"/>
+      <c r="D11" s="30"/>
+      <c r="E11" s="30"/>
+      <c r="F11" s="30"/>
+      <c r="G11" s="30"/>
+      <c r="H11" s="30"/>
       <c r="I11" s="18"/>
       <c r="J11" s="18"/>
     </row>
-    <row r="12" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A12" s="31"/>
+    <row r="12" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A12" s="28"/>
       <c r="B12" s="16"/>
-      <c r="C12" s="32"/>
+      <c r="C12" s="29"/>
       <c r="D12" s="17"/>
       <c r="E12" s="17"/>
       <c r="F12" s="17"/>
-      <c r="G12" s="33"/>
+      <c r="G12" s="30"/>
       <c r="H12" s="17"/>
-      <c r="I12" s="34"/>
+      <c r="I12" s="31"/>
       <c r="J12" s="18"/>
     </row>
-    <row r="13" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="13" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A13" s="16"/>
       <c r="B13" s="16"/>
       <c r="C13" s="16"/>
@@ -942,7 +924,7 @@
       <c r="I13" s="18"/>
       <c r="J13" s="18"/>
     </row>
-    <row r="14" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="14" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A14" s="16"/>
       <c r="B14" s="16"/>
       <c r="C14" s="16"/>
@@ -954,7 +936,7 @@
       <c r="I14" s="18"/>
       <c r="J14" s="18"/>
     </row>
-    <row r="15" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="15" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A15" s="16"/>
       <c r="B15" s="16"/>
       <c r="C15" s="16"/>
@@ -963,10 +945,10 @@
       <c r="F15" s="17"/>
       <c r="G15" s="17"/>
       <c r="H15" s="17"/>
-      <c r="I15" s="34"/>
+      <c r="I15" s="31"/>
       <c r="J15" s="18"/>
     </row>
-    <row r="16" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="16" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A16" s="16"/>
       <c r="B16" s="16"/>
       <c r="C16" s="16"/>
@@ -978,7 +960,7 @@
       <c r="I16" s="18"/>
       <c r="J16" s="18"/>
     </row>
-    <row r="17" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="17" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A17" s="16"/>
       <c r="B17" s="16"/>
       <c r="C17" s="16"/>
@@ -988,9 +970,9 @@
       <c r="G17" s="17"/>
       <c r="H17" s="17"/>
       <c r="I17" s="18"/>
-      <c r="J17" s="34"/>
-    </row>
-    <row r="18" spans="1:10" x14ac:dyDescent="0.25">
+      <c r="J17" s="31"/>
+    </row>
+    <row r="18" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A18" s="16"/>
       <c r="B18" s="16"/>
       <c r="C18" s="16"/>
@@ -1002,7 +984,7 @@
       <c r="I18" s="18"/>
       <c r="J18" s="18"/>
     </row>
-    <row r="19" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="19" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A19" s="16"/>
       <c r="B19" s="16"/>
       <c r="C19" s="16"/>
@@ -1014,7 +996,7 @@
       <c r="I19" s="18"/>
       <c r="J19" s="18"/>
     </row>
-    <row r="20" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="20" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A20" s="19"/>
       <c r="B20" s="19"/>
       <c r="C20" s="19"/>
@@ -1026,7 +1008,7 @@
       <c r="I20" s="21"/>
       <c r="J20" s="21"/>
     </row>
-    <row r="21" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="21" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A21" s="19"/>
       <c r="B21" s="19"/>
       <c r="C21" s="19"/>
@@ -1038,7 +1020,7 @@
       <c r="I21" s="21"/>
       <c r="J21" s="21"/>
     </row>
-    <row r="22" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="22" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A22" s="19"/>
       <c r="B22" s="19"/>
       <c r="C22" s="19"/>
@@ -1050,7 +1032,7 @@
       <c r="I22" s="21"/>
       <c r="J22" s="21"/>
     </row>
-    <row r="23" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="23" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A23" s="22"/>
       <c r="B23" s="22"/>
       <c r="C23" s="22"/>
@@ -1062,7 +1044,7 @@
       <c r="I23" s="21"/>
       <c r="J23" s="21"/>
     </row>
-    <row r="24" spans="1:10" x14ac:dyDescent="0.25">
+    <row r="24" spans="1:10" x14ac:dyDescent="0.3">
       <c r="A24" s="23"/>
       <c r="B24" s="23"/>
       <c r="C24" s="23"/>
@@ -1074,7 +1056,7 @@
       <c r="I24" s="24"/>
       <c r="J24" s="24"/>
     </row>
-    <row r="25" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
+    <row r="25" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
       <c r="A25" s="25"/>
       <c r="B25" s="25"/>
       <c r="C25" s="25"/>
@@ -1086,119 +1068,104 @@
       <c r="I25" s="26"/>
       <c r="J25" s="26"/>
     </row>
-    <row r="26" spans="1:10" ht="15.75" x14ac:dyDescent="0.25">
-      <c r="A26" s="27"/>
-      <c r="B26" s="28"/>
-      <c r="C26" s="28"/>
-      <c r="D26" s="28"/>
-      <c r="E26" s="28"/>
-      <c r="F26" s="28"/>
-      <c r="G26" s="28"/>
-      <c r="H26" s="28"/>
-      <c r="I26" s="28"/>
-      <c r="J26" s="28"/>
-    </row>
-    <row r="27" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A27" s="28"/>
-      <c r="B27" s="28"/>
-      <c r="C27" s="28"/>
-      <c r="D27" s="28"/>
-      <c r="E27" s="28"/>
-      <c r="F27" s="28"/>
-      <c r="G27" s="28"/>
-      <c r="H27" s="28"/>
-      <c r="I27" s="28"/>
-      <c r="J27" s="28"/>
-    </row>
-    <row r="28" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A28" s="29"/>
-      <c r="B28" s="29"/>
-      <c r="C28" s="29"/>
-      <c r="D28" s="29"/>
-      <c r="E28" s="29"/>
-      <c r="F28" s="29"/>
-      <c r="G28" s="29"/>
-      <c r="H28" s="29"/>
-      <c r="I28" s="29"/>
-      <c r="J28" s="29"/>
-    </row>
-    <row r="29" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A29" s="29"/>
-      <c r="B29" s="29"/>
-      <c r="C29" s="29"/>
-      <c r="D29" s="29"/>
-      <c r="E29" s="29"/>
-      <c r="F29" s="29"/>
-      <c r="G29" s="29"/>
-      <c r="H29" s="29"/>
-      <c r="I29" s="29"/>
-      <c r="J29" s="29"/>
-    </row>
-    <row r="30" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A30" s="29"/>
-      <c r="B30" s="29"/>
-      <c r="C30" s="29"/>
-      <c r="D30" s="29"/>
-      <c r="E30" s="29"/>
-      <c r="F30" s="29"/>
-      <c r="G30" s="29"/>
-      <c r="H30" s="29"/>
-      <c r="I30" s="29"/>
-      <c r="J30" s="29"/>
-    </row>
-    <row r="31" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A31" s="29"/>
-      <c r="B31" s="29"/>
-      <c r="C31" s="29"/>
-      <c r="D31" s="29"/>
-      <c r="E31" s="29"/>
-      <c r="F31" s="29"/>
-      <c r="G31" s="29"/>
-      <c r="H31" s="29"/>
-      <c r="I31" s="29"/>
-      <c r="J31" s="29"/>
-    </row>
-    <row r="32" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A32" s="29"/>
-      <c r="B32" s="29"/>
-      <c r="C32" s="29"/>
-      <c r="D32" s="29"/>
-      <c r="E32" s="29"/>
-      <c r="F32" s="29"/>
-      <c r="G32" s="29"/>
-      <c r="H32" s="29"/>
-      <c r="I32" s="29"/>
-      <c r="J32" s="29"/>
-    </row>
-    <row r="33" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A33" s="29"/>
-      <c r="B33" s="29"/>
-      <c r="C33" s="29"/>
-      <c r="D33" s="29"/>
-      <c r="E33" s="29"/>
-      <c r="F33" s="29"/>
-      <c r="G33" s="29"/>
-      <c r="H33" s="29"/>
-      <c r="I33" s="29"/>
-      <c r="J33" s="29"/>
-    </row>
-    <row r="34" spans="1:10" x14ac:dyDescent="0.25">
-      <c r="A34" s="35" t="s">
-        <v>4</v>
-      </c>
-      <c r="B34" s="35"/>
-      <c r="C34" s="35"/>
-      <c r="D34" s="35"/>
-      <c r="E34" s="35"/>
-      <c r="F34" s="35"/>
-      <c r="G34" s="35"/>
-      <c r="H34" s="35"/>
-      <c r="I34" s="29"/>
-      <c r="J34" s="29"/>
+    <row r="26" spans="1:10" ht="15.6" x14ac:dyDescent="0.3">
+      <c r="A26" s="25"/>
+      <c r="B26" s="26"/>
+      <c r="C26" s="26"/>
+      <c r="D26" s="26"/>
+      <c r="E26" s="26"/>
+      <c r="F26" s="26"/>
+      <c r="G26" s="26"/>
+      <c r="H26" s="26"/>
+      <c r="I26" s="26"/>
+      <c r="J26" s="26"/>
+    </row>
+    <row r="27" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A27" s="26"/>
+      <c r="B27" s="26"/>
+      <c r="C27" s="26"/>
+      <c r="D27" s="26"/>
+      <c r="E27" s="26"/>
+      <c r="F27" s="26"/>
+      <c r="G27" s="26"/>
+      <c r="H27" s="26"/>
+      <c r="I27" s="26"/>
+      <c r="J27" s="26"/>
+    </row>
+    <row r="28" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A28" s="26"/>
+      <c r="B28" s="26"/>
+      <c r="C28" s="26"/>
+      <c r="D28" s="26"/>
+      <c r="E28" s="26"/>
+      <c r="F28" s="26"/>
+      <c r="G28" s="26"/>
+      <c r="H28" s="26"/>
+      <c r="I28" s="26"/>
+      <c r="J28" s="26"/>
+    </row>
+    <row r="29" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A29" s="26"/>
+      <c r="B29" s="26"/>
+      <c r="C29" s="26"/>
+      <c r="D29" s="26"/>
+      <c r="E29" s="26"/>
+      <c r="F29" s="26"/>
+      <c r="G29" s="26"/>
+      <c r="H29" s="26"/>
+      <c r="I29" s="26"/>
+      <c r="J29" s="26"/>
+    </row>
+    <row r="30" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A30" s="26"/>
+      <c r="B30" s="26"/>
+      <c r="C30" s="26"/>
+      <c r="D30" s="26"/>
+      <c r="E30" s="26"/>
+      <c r="F30" s="26"/>
+      <c r="G30" s="26"/>
+      <c r="H30" s="26"/>
+      <c r="I30" s="26"/>
+      <c r="J30" s="26"/>
+    </row>
+    <row r="31" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A31" s="26"/>
+      <c r="B31" s="26"/>
+      <c r="C31" s="26"/>
+      <c r="D31" s="26"/>
+      <c r="E31" s="26"/>
+      <c r="F31" s="26"/>
+      <c r="G31" s="26"/>
+      <c r="H31" s="26"/>
+      <c r="I31" s="26"/>
+      <c r="J31" s="26"/>
+    </row>
+    <row r="32" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A32" s="26"/>
+      <c r="B32" s="26"/>
+      <c r="C32" s="26"/>
+      <c r="D32" s="26"/>
+      <c r="E32" s="26"/>
+      <c r="F32" s="26"/>
+      <c r="G32" s="26"/>
+      <c r="H32" s="26"/>
+      <c r="I32" s="26"/>
+      <c r="J32" s="26"/>
+    </row>
+    <row r="33" spans="1:10" x14ac:dyDescent="0.3">
+      <c r="A33" s="26"/>
+      <c r="B33" s="26"/>
+      <c r="C33" s="26"/>
+      <c r="D33" s="26"/>
+      <c r="E33" s="26"/>
+      <c r="F33" s="26"/>
+      <c r="G33" s="26"/>
+      <c r="H33" s="26"/>
+      <c r="I33" s="26"/>
+      <c r="J33" s="26"/>
     </row>
   </sheetData>
-  <mergeCells count="11">
-    <mergeCell ref="A34:H34"/>
+  <mergeCells count="10">
     <mergeCell ref="A7:A10"/>
     <mergeCell ref="B7:B10"/>
     <mergeCell ref="C7:C10"/>

</xml_diff>

<commit_message>
Combinacion de celdas libro diario corregido
</commit_message>
<xml_diff>
--- a/app/templates/contable/plantillas/L,D.xlsx
+++ b/app/templates/contable/plantillas/L,D.xlsx
@@ -5,10 +5,10 @@
   <workbookPr/>
   <mc:AlternateContent xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006">
     <mc:Choice Requires="x15">
-      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="C:\Users\angel\OneDrive\Imágenes\Escritorio\"/>
+      <x15ac:absPath xmlns:x15ac="http://schemas.microsoft.com/office/spreadsheetml/2010/11/ac" url="D:\LPT ANGEL\USAT\8º Ciclo\INGENIERÍA Y CALIDAD DE SOFTWARE\CONTABILIDAD_PROYECTO2\CONTABILIDAD_PROYECTO\app\templates\contable\plantillas\"/>
     </mc:Choice>
   </mc:AlternateContent>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{A9A6DEBD-5A02-4485-8D41-5BAF5394F0E0}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{889DB162-7807-483A-B46C-CE63343574B7}" xr6:coauthVersionLast="47" xr6:coauthVersionMax="47" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
   <bookViews>
     <workbookView xWindow="-108" yWindow="-108" windowWidth="23256" windowHeight="12456" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
   </bookViews>
@@ -72,9 +72,6 @@
     <t xml:space="preserve">                       MOVIMIENTO</t>
   </si>
   <si>
-    <t>N° CORREL. L.M</t>
-  </si>
-  <si>
     <t>N° DOCUMENTO SUSTENTAT.</t>
   </si>
   <si>
@@ -82,6 +79,9 @@
   </si>
   <si>
     <t>HABER</t>
+  </si>
+  <si>
+    <t>N° CORRELATIVO</t>
   </si>
 </sst>
 </file>
@@ -712,8 +712,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
   <dimension ref="A1:J33"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A26" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
-      <selection activeCell="D27" sqref="D27"/>
+    <sheetView tabSelected="1" zoomScale="110" zoomScaleNormal="110" workbookViewId="0">
+      <selection activeCell="H12" sqref="H11:H12"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="14.4" x14ac:dyDescent="0.3"/>
@@ -842,10 +842,10 @@
         <v>11</v>
       </c>
       <c r="E8" s="32" t="s">
+        <v>18</v>
+      </c>
+      <c r="F8" s="32" t="s">
         <v>15</v>
-      </c>
-      <c r="F8" s="32" t="s">
-        <v>16</v>
       </c>
       <c r="G8" s="38" t="s">
         <v>7</v>
@@ -882,10 +882,10 @@
       <c r="G10" s="40"/>
       <c r="H10" s="40"/>
       <c r="I10" s="14" t="s">
+        <v>16</v>
+      </c>
+      <c r="J10" s="15" t="s">
         <v>17</v>
-      </c>
-      <c r="J10" s="15" t="s">
-        <v>18</v>
       </c>
     </row>
     <row r="11" spans="1:10" x14ac:dyDescent="0.3">

</xml_diff>